<commit_message>
Add issue number to group message captions
</commit_message>
<xml_diff>
--- a/conclusions.xlsx
+++ b/conclusions.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
@@ -1507,6 +1507,51 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>01120015455</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>385</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>02.12.2025</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Тест</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>1 000</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Oleg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>